<commit_message>
cambios en prescripcion y caracterizacion
</commit_message>
<xml_diff>
--- a/variables mejores 400 puntos.xlsx
+++ b/variables mejores 400 puntos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\api_maestria_colegios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A09B668-FB2A-4FE4-A3EB-90749370B9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC38A62-7CFD-42EA-A4A4-B0DDDCE4EEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E5E3C285-7207-4CE0-BCC4-E9A2D04D2167}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
     <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="120">
   <si>
     <t>ESTU_TIPODOCUMENTO</t>
   </si>
@@ -324,9 +324,6 @@
     <t>porcenra mejores400</t>
   </si>
   <si>
-    <t>No sabe no aplica</t>
-  </si>
-  <si>
     <t>ninguno</t>
   </si>
   <si>
@@ -387,7 +384,28 @@
     <t>Estrategia: aumentar a minimo una hora diaria de lectura</t>
   </si>
   <si>
-    <t>Mayor o igual  a 60%, se suma las categorias de entre 30 y 60 minutos, 1 y 2 horas, mas de horas</t>
+    <t>Ninguno no aplica</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>Umbral: si la proporcion de estudiantes no supera el 60% con minomo 30 minutos de lectura al día Mayor o igual  a 60%, se suma las categorias de entre 30 y 60 minutos, 1 y 2 horas, mas de horas</t>
+  </si>
+  <si>
+    <t>Umbral: si el porcentaje de madres No supera el 90% con minimo tecnico para arriba se propone mejora</t>
+  </si>
+  <si>
+    <t>Estrategia:fomentar acceso educacion minomo técnica</t>
+  </si>
+  <si>
+    <t>actual (25,68,8)</t>
+  </si>
+  <si>
+    <t>Umbra: minimo el 80% de las familias deben tener mas de 25 libros</t>
+  </si>
+  <si>
+    <t>Estrategia: campaña de aumento de libros en casa.</t>
   </si>
 </sst>
 </file>
@@ -467,890 +485,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>mayor400puntos!$C$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Frecuencia</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>mayor400puntos!$B$21:$B$25</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Entre 30 y 60 minutos</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30 minutos o menos</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Entre 1 y 2 horas</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>No leo por entretenimiento</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mas de 2 horas</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>mayor400puntos!$C$21:$C$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>157</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7615-4349-9DA2-3670A95C10DE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1025622847"/>
-        <c:axId val="1025607455"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1025622847"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1025607455"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1025607455"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1025622847"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC67C2B5-8C3C-4FD8-BE89-B86AA1F05CB1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24544,7 +23678,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3E89500F-FF89-43E0-8620-2A280FD11D34}" name="TablaDinámica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3E89500F-FF89-43E0-8620-2A280FD11D34}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:C8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="48">
     <pivotField showAll="0"/>
@@ -25117,15 +24251,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37E8154-F76D-42E2-B8B1-6F054F83B93D}">
-  <dimension ref="A3:H88"/>
+  <dimension ref="A3:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F21" activeCellId="2" sqref="F23 F25 F21"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -25136,7 +24270,7 @@
         <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -25181,7 +24315,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
         <v>55</v>
@@ -25221,7 +24355,7 @@
         <v>0.26684456304202803</v>
       </c>
       <c r="H21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -25268,7 +24402,7 @@
         <v>0.11874583055370247</v>
       </c>
       <c r="H23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -25330,6 +24464,9 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
       <c r="B29" t="s">
         <v>59</v>
       </c>
@@ -25349,6 +24486,9 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
       <c r="B30" t="s">
         <v>62</v>
       </c>
@@ -25366,8 +24506,14 @@
         <f t="shared" ref="F30:F39" si="3">+E30/SUM($E$29:$E$38)</f>
         <v>4.6153846153846156E-2</v>
       </c>
+      <c r="H30" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>8</v>
+      </c>
       <c r="B31" t="s">
         <v>65</v>
       </c>
@@ -25385,8 +24531,14 @@
         <f t="shared" si="3"/>
         <v>0.21672240802675585</v>
       </c>
+      <c r="H31" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
       <c r="B32" t="s">
         <v>67</v>
       </c>
@@ -25405,7 +24557,10 @@
         <v>0.21270903010033446</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
       <c r="B33" t="s">
         <v>60</v>
       </c>
@@ -25424,7 +24579,10 @@
         <v>6.0869565217391307E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11</v>
+      </c>
       <c r="B34" t="s">
         <v>68</v>
       </c>
@@ -25443,7 +24601,10 @@
         <v>4.6822742474916385E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>9</v>
+      </c>
       <c r="B35" t="s">
         <v>66</v>
       </c>
@@ -25462,7 +24623,10 @@
         <v>4.9498327759197325E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>7</v>
+      </c>
       <c r="B36" t="s">
         <v>64</v>
       </c>
@@ -25481,7 +24645,10 @@
         <v>1.137123745819398E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>4</v>
+      </c>
       <c r="B37" t="s">
         <v>61</v>
       </c>
@@ -25500,7 +24667,10 @@
         <v>3.8795986622073578E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6</v>
+      </c>
       <c r="B38" t="s">
         <v>63</v>
       </c>
@@ -25519,9 +24689,12 @@
         <v>1.6722408026755852E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>113</v>
+      </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="5"/>
@@ -25533,7 +24706,7 @@
         <v>2.6755852842809363E-3</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>72</v>
       </c>
@@ -25547,7 +24720,10 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
       <c r="B42" t="s">
         <v>77</v>
       </c>
@@ -25565,8 +24741,14 @@
         <f>+E42/SUM($E$42:$E$45)</f>
         <v>0.3255503669112742</v>
       </c>
+      <c r="H42" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3</v>
+      </c>
       <c r="B43" t="s">
         <v>78</v>
       </c>
@@ -25584,8 +24766,14 @@
         <f t="shared" ref="F43:F45" si="4">+E43/SUM($E$42:$E$45)</f>
         <v>0.11741160773849232</v>
       </c>
+      <c r="H43" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
       <c r="B44" t="s">
         <v>76</v>
       </c>
@@ -25603,8 +24791,14 @@
         <f t="shared" si="4"/>
         <v>0.32755170113408938</v>
       </c>
+      <c r="I44" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
       <c r="B45" t="s">
         <v>75</v>
       </c>
@@ -25623,7 +24817,7 @@
         <v>0.22948632421614409</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>80</v>
       </c>
@@ -25851,7 +25045,7 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="5"/>
@@ -25981,24 +25175,24 @@
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C69" t="s">
         <v>58</v>
       </c>
       <c r="D69" t="s">
+        <v>98</v>
+      </c>
+      <c r="E69" t="s">
         <v>99</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>100</v>
-      </c>
-      <c r="F69" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C70" s="3">
         <v>349</v>
@@ -26017,7 +25211,7 @@
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C71" s="3">
         <v>36</v>
@@ -26036,7 +25230,7 @@
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C72" s="3">
         <v>11</v>
@@ -26055,7 +25249,7 @@
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C73" s="3">
         <v>2</v>
@@ -26074,13 +25268,13 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C75" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D75" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E75" t="s">
         <v>83</v>
@@ -26091,7 +25285,7 @@
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C76">
         <v>4</v>
@@ -26110,7 +25304,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C77">
         <v>394</v>
@@ -26129,13 +25323,13 @@
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C80" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D80" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E80" t="s">
         <v>83</v>
@@ -26146,7 +25340,7 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C81">
         <v>2</v>
@@ -26165,7 +25359,7 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C82">
         <v>396</v>
@@ -26184,24 +25378,24 @@
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C84" t="s">
         <v>56</v>
       </c>
       <c r="D84" t="s">
+        <v>107</v>
+      </c>
+      <c r="E84" t="s">
+        <v>99</v>
+      </c>
+      <c r="F84" t="s">
         <v>108</v>
-      </c>
-      <c r="E84" t="s">
-        <v>100</v>
-      </c>
-      <c r="F84" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C85" s="3">
         <v>293</v>
@@ -26220,7 +25414,7 @@
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C86" s="3">
         <v>64</v>
@@ -26239,7 +25433,7 @@
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C87" s="3">
         <v>36</v>
@@ -26258,7 +25452,7 @@
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C88" s="3">
         <v>5</v>
@@ -26277,7 +25471,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
cambios de caracterizacion se incluyen fallos
</commit_message>
<xml_diff>
--- a/variables mejores 400 puntos.xlsx
+++ b/variables mejores 400 puntos.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\api_maestria_colegios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D76EF5-4A6E-4532-992D-E199D119078A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0710D90A-C8DA-43EC-B7FA-59A86C48B905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E5E3C285-7207-4CE0-BCC4-E9A2D04D2167}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{E5E3C285-7207-4CE0-BCC4-E9A2D04D2167}"/>
   </bookViews>
   <sheets>
     <sheet name="mayor400puntos" sheetId="2" r:id="rId1"/>
-    <sheet name="todos" sheetId="1" r:id="rId2"/>
-    <sheet name="anamayor430" sheetId="4" r:id="rId3"/>
-    <sheet name="mayor430" sheetId="3" r:id="rId4"/>
+    <sheet name="variablesumbral" sheetId="5" r:id="rId2"/>
+    <sheet name="todos" sheetId="1" r:id="rId3"/>
+    <sheet name="anamayor430" sheetId="4" r:id="rId4"/>
+    <sheet name="mayor430" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mayor400puntos!$B$84:$F$88</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">mayor430!$A$1:$AV$59</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">todos!$A$1:$AV$399</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">mayor430!$A$1:$AV$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">todos!$A$1:$AV$399</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="152">
   <si>
     <t>ESTU_TIPODOCUMENTO</t>
   </si>
@@ -405,9 +406,6 @@
     <t>Estrategia: campaña de aumento de libros en casa.</t>
   </si>
   <si>
-    <t>Umbral: si el porcentaje de madres No supera el 88% con minimo tecnico para arriba se propone mejora</t>
-  </si>
-  <si>
     <t>Estrategia: máximo de horas de trabajo por semana a 20 horas</t>
   </si>
   <si>
@@ -445,6 +443,66 @@
   </si>
   <si>
     <t>Estrategia: aumentar frecuencia de leche derivados a minimo 3 veces por semana</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Dedicación de lectura diaria</t>
+  </si>
+  <si>
+    <t>Nivel educativo de la madre</t>
+  </si>
+  <si>
+    <t>Número de libros en casa.</t>
+  </si>
+  <si>
+    <t>Menos del 60% de los estudiantes lee más de 30 minutos por día</t>
+  </si>
+  <si>
+    <t>Menos del 90% de las madres de los estudiantes cuentan con mínimo un técnico</t>
+  </si>
+  <si>
+    <t>Menos del 80% de las familias cuentan con más de 25 libros en casa</t>
+  </si>
+  <si>
+    <t>Umbral por colegio</t>
+  </si>
+  <si>
+    <t>Se detecta un fallo: Baja cantidad de libros en casa.</t>
+  </si>
+  <si>
+    <t>Nivel educativo del padre</t>
+  </si>
+  <si>
+    <t>Umbral: si el porcentaje de padres No supera el 88% con minimo tecnico para arriba se propone mejora</t>
+  </si>
+  <si>
+    <t>Menos del 88% de los padres de los estudiantes cuentan con mínimo un técnico</t>
+  </si>
+  <si>
+    <t>Se detecta un fallo: Nivel educativo de las madres.</t>
+  </si>
+  <si>
+    <t>Se detecta un fallo: Nivel educativo de los padres.</t>
+  </si>
+  <si>
+    <t>Se detecta un fallo: Baja dedicación de lectura diaria.</t>
+  </si>
+  <si>
+    <t>Horas de trabajo por semana del estudiante</t>
+  </si>
+  <si>
+    <t>Más del 6% de los estudiantes trabaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se detecta un fallo: </t>
+  </si>
+  <si>
+    <t>Mejora detectada</t>
+  </si>
+  <si>
+    <t>Más del 1% no tiene computador</t>
   </si>
 </sst>
 </file>
@@ -497,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -508,6 +566,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -24292,8 +24351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37E8154-F76D-42E2-B8B1-6F054F83B93D}">
   <dimension ref="A3:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24441,7 +24500,7 @@
         <v>0.11874583055370247</v>
       </c>
       <c r="H23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -24917,7 +24976,7 @@
         <v>0.23324396782841822</v>
       </c>
       <c r="H50" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -25177,7 +25236,7 @@
         <v>0.8325550366911274</v>
       </c>
       <c r="H63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -25224,7 +25283,7 @@
         <v>3.7358238825883926E-2</v>
       </c>
       <c r="H65" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -25314,10 +25373,10 @@
         <v>0.61174116077384921</v>
       </c>
       <c r="H70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -25364,7 +25423,7 @@
         <v>9.0060040026684454E-2</v>
       </c>
       <c r="H72" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -25428,10 +25487,10 @@
         <v>6.6044029352901934E-2</v>
       </c>
       <c r="H76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -25456,10 +25515,10 @@
         <v>0.93395597064709801</v>
       </c>
       <c r="H77" t="s">
+        <v>126</v>
+      </c>
+      <c r="I77" t="s">
         <v>127</v>
-      </c>
-      <c r="I77" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -25501,10 +25560,10 @@
         <v>2.6684456304202801E-2</v>
       </c>
       <c r="H81" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I81" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -25529,10 +25588,10 @@
         <v>0.9733155436957972</v>
       </c>
       <c r="H82" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I82" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -25596,10 +25655,10 @@
         <v>0.28285523682454972</v>
       </c>
       <c r="H86" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I86" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -25646,7 +25705,7 @@
         <v>4.6030687124749836E-2</v>
       </c>
       <c r="H88" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -25655,6 +25714,99 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56978C1B-257C-4AD7-A4D1-01B32B926F66}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3338BF8E-61C6-4653-8DB3-20124CB53F5B}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AV399"/>
@@ -83931,7 +84083,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B79C729-EA48-4B8D-9B86-7E0DA9BEB5E9}">
   <dimension ref="A3:B18"/>
   <sheetViews>
@@ -84046,7 +84198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C293690F-3DFE-49F6-934A-1C5FF0055E16}">
   <dimension ref="A1:AV59"/>
   <sheetViews>

</xml_diff>